<commit_message>
wetland data with notes about issues
</commit_message>
<xml_diff>
--- a/Wetlands/Wetland data.xlsx
+++ b/Wetlands/Wetland data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymad138\Documents\Ecuador2022\Wetlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EF0704-1656-4A7A-850C-E0D8C4E8ACD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD78843-7F3B-4F92-86B5-AC6F959B6D5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="6280" xr2:uid="{94E7109B-EF61-4772-AC1F-D142A6519923}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Wetland</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Plot looks right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphs do not show on this </t>
+  </si>
+  <si>
+    <t>The graph doesn’t show up</t>
+  </si>
+  <si>
+    <t>Date in file says 7-13, while the file name says 7-8</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF46F0BE-CA28-4568-AEEA-82D636B2E98E}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -946,6 +955,10 @@
       <c r="C29" s="7">
         <v>44741</v>
       </c>
+      <c r="D29" s="12"/>
+      <c r="F29" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
@@ -957,6 +970,10 @@
       <c r="C30" s="7">
         <v>44741</v>
       </c>
+      <c r="D30" s="12"/>
+      <c r="F30" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
@@ -968,6 +985,12 @@
       <c r="C31" s="7">
         <v>44741</v>
       </c>
+      <c r="D31" s="12">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="E31" s="6">
+        <v>248.88140000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
@@ -986,7 +1009,7 @@
         <v>593.62710000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>4</v>
       </c>
@@ -1003,7 +1026,7 @@
         <v>664.72879999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>4</v>
       </c>
@@ -1020,7 +1043,7 @@
         <v>653.79660000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1037,7 +1060,7 @@
         <v>395.83049999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1054,7 +1077,7 @@
         <v>492.61020000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1071,7 +1094,7 @@
         <v>492.35590000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1088,7 +1111,7 @@
         <v>756.20699999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
@@ -1105,7 +1128,7 @@
         <v>681.66629999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1122,7 +1145,7 @@
         <v>669.47460000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1139,7 +1162,7 @@
         <v>459.22030000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1156,7 +1179,7 @@
         <v>843.44069999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1173,7 +1196,7 @@
         <v>694.81359999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1190,7 +1213,7 @@
         <v>642.01689999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>6</v>
       </c>
@@ -1200,8 +1223,11 @@
       <c r="C45" s="7">
         <v>44742</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F45" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>6</v>
       </c>
@@ -1211,8 +1237,11 @@
       <c r="C46" s="7">
         <v>44742</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F46" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>6</v>
       </c>
@@ -1222,8 +1251,11 @@
       <c r="C47" s="7">
         <v>44742</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F47" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="8">
         <v>6</v>
       </c>
@@ -1233,8 +1265,11 @@
       <c r="C48" s="9">
         <v>44753</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F48" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="8">
         <v>6</v>
       </c>
@@ -1244,8 +1279,11 @@
       <c r="C49" s="9">
         <v>44753</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F49" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="8">
         <v>6</v>
       </c>
@@ -1255,8 +1293,11 @@
       <c r="C50" s="9">
         <v>44753</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
@@ -1273,7 +1314,7 @@
         <v>394.05079999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1290,7 +1331,7 @@
         <v>434.89830000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>6</v>
       </c>
@@ -1307,7 +1348,7 @@
         <v>393.11860000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>7</v>
       </c>
@@ -1317,8 +1358,11 @@
       <c r="C54" s="7">
         <v>44742</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F54" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>7</v>
       </c>
@@ -1328,8 +1372,11 @@
       <c r="C55" s="7">
         <v>44742</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F55" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>7</v>
       </c>
@@ -1339,8 +1386,11 @@
       <c r="C56" s="7">
         <v>44742</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F56" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="8">
         <v>7</v>
       </c>
@@ -1350,8 +1400,11 @@
       <c r="C57" s="9">
         <v>44753</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F57" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="8">
         <v>7</v>
       </c>
@@ -1361,8 +1414,11 @@
       <c r="C58" s="9">
         <v>44753</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F58" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="8">
         <v>7</v>
       </c>
@@ -1372,8 +1428,11 @@
       <c r="C59" s="9">
         <v>44753</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>7</v>
       </c>
@@ -1390,7 +1449,7 @@
         <v>452.10169999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>7</v>
       </c>
@@ -1407,7 +1466,7 @@
         <v>491.16950000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>7</v>
       </c>
@@ -1424,7 +1483,7 @@
         <v>452.18639999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -1441,7 +1500,7 @@
         <v>9397.9320000000007</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -1458,7 +1517,7 @@
         <v>7530.3050000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -1475,7 +1534,7 @@
         <v>3354.39</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
@@ -1492,7 +1551,7 @@
         <v>10517.98</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>8</v>
       </c>
@@ -1509,7 +1568,7 @@
         <v>7493.1189999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>8</v>
       </c>
@@ -1526,7 +1585,7 @@
         <v>6369.29</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>8</v>
       </c>
@@ -1543,7 +1602,7 @@
         <v>5026.1189999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>8</v>
       </c>
@@ -1560,7 +1619,7 @@
         <v>5242.5590000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>8</v>
       </c>
@@ -1577,7 +1636,7 @@
         <v>4312.1530000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>9</v>
       </c>
@@ -1594,7 +1653,7 @@
         <v>4119.2879999999996</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10">
         <v>9</v>
       </c>
@@ -1604,8 +1663,11 @@
       <c r="C73" s="11">
         <v>44750</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G73" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="10">
         <v>9</v>
       </c>
@@ -1616,7 +1678,7 @@
         <v>44750</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10">
         <v>9</v>
       </c>
@@ -1627,7 +1689,7 @@
         <v>44750</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>9</v>
       </c>
@@ -1644,7 +1706,7 @@
         <v>3202.6950000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
@@ -1661,7 +1723,7 @@
         <v>1238.9490000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>10</v>
       </c>
@@ -1678,7 +1740,7 @@
         <v>1888.932</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>10</v>
       </c>
@@ -1695,7 +1757,7 @@
         <v>2716.78</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>10</v>
       </c>
@@ -1858,6 +1920,12 @@
       <c r="C89" s="7">
         <v>44748</v>
       </c>
+      <c r="D89" s="12">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="E89" s="6">
+        <v>1154.627</v>
+      </c>
     </row>
     <row r="90" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
@@ -1869,6 +1937,12 @@
       <c r="C90" s="7">
         <v>44748</v>
       </c>
+      <c r="D90" s="12">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="E90" s="6">
+        <v>1131.7460000000001</v>
+      </c>
     </row>
     <row r="91" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
@@ -1879,6 +1953,12 @@
       </c>
       <c r="C91" s="7">
         <v>44748</v>
+      </c>
+      <c r="D91" s="12">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="E91" s="6">
+        <v>1113.78</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated wetland sata and temp
</commit_message>
<xml_diff>
--- a/Wetlands/Wetland data.xlsx
+++ b/Wetlands/Wetland data.xlsx
@@ -8,72 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymad138\Documents\Ecuador2022\Wetlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7C3F6-F617-412E-953B-7E395C0D9F1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B163DE36-DC91-470B-9384-73710C9C3D92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="6280" activeTab="1" xr2:uid="{94E7109B-EF61-4772-AC1F-D142A6519923}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="6280" xr2:uid="{94E7109B-EF61-4772-AC1F-D142A6519923}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$11:$E$19</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$54:$E$59</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$E$72:$E$76</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$E$29:$E$30</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$E$31:$E$37</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$E$63:$E$71</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$89:$E$97</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$3:$E$10</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$E$89:$E$97</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$E$86:$E$88</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$45:$E$50</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$60:$E$62</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$E$51:$E$53</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$E$89:$E$97</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$E$86:$E$88</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$E$72:$E$76</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$E$20</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$E$21:$E$28</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$E$3:$E$10</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$E$89:$E$97</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$E$63:$E$71</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$77:$E$85</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$E$86:$E$88</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$E$86:$E$88</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$E$77:$E$85</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$E$11:$E$19</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$E$89:$E$97</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$E$29:$E$30</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$E$31:$E$37</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$E$29:$E$30</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$E$31:$E$37</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$E$54:$E$59</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$86:$E$88</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$E$60:$E$62</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$E$45:$E$50</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$E$51:$E$53</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$E$45:$E$50</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$E$51:$E$53</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$E$54:$E$59</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$E$60:$E$62</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$E$20</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$E$21:$E$28</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$E$72:$E$76</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$45:$E$50</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$E$3:$E$10</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$E$38:$E$44</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$E$11:$E$19</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$E$77:$E$85</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$E$38:$E$44</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$E$63:$E$71</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$51:$E$53</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$38:$E$44</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$21:$E$28</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$84:$E$86</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$20</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$E$61:$E$69</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$E$38:$E$44</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$E$87:$E$95</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$E$29:$E$30</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$31:$E$37</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$E$70:$E$74</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$75:$E$83</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$21:$E$28</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$11:$E$19</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$45:$E$48</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$49:$E$51</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$3:$E$10</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$52:$E$57</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$58:$E$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Wetland</t>
   </si>
@@ -123,16 +83,10 @@
     <t>11:18-19</t>
   </si>
   <si>
-    <t>The plot does not exist</t>
-  </si>
-  <si>
     <t>10:38-10:39</t>
   </si>
   <si>
     <t>The plot is just flat and doesn’t look right</t>
-  </si>
-  <si>
-    <t>Plot looks right</t>
   </si>
   <si>
     <t xml:space="preserve">Graphs do not show on this </t>
@@ -199,6 +153,9 @@
   </si>
   <si>
     <t xml:space="preserve">Range </t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -293,7 +250,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -331,8 +288,8 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F0080D1D-1343-46BA-B782-71978689C18A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.15</cx:f>
-              <cx:v/>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v>NA</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -347,7 +304,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -389,7 +346,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -437,7 +394,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -479,7 +436,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -527,7 +484,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -569,7 +526,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -607,8 +564,8 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3C260FED-A921-41EB-A4F1-B5F8FCAD3EFD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
-              <cx:v/>
+              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:v>NA</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -623,7 +580,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -665,7 +622,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -713,7 +670,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -755,7 +712,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -793,7 +750,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{0E07CA08-7672-4C11-A68A-88695AA7DEA7}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -809,7 +766,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -851,7 +808,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -899,7 +856,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -941,7 +898,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -979,8 +936,8 @@
         <cx:series layoutId="boxWhisker" uniqueId="{939C9611-904F-4791-8AE2-4C41FA502AAB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
-              <cx:v/>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>430.7458</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -995,7 +952,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000" min="0"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -1037,7 +994,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1075,7 +1032,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8A987424-C800-4688-9AFA-F9318EC37BD4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -1091,7 +1048,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000" min="0"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -1133,7 +1090,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1223,7 +1180,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1271,7 +1228,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -1313,7 +1270,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1361,7 +1318,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling/>
+        <cx:valScaling max="12000"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -9296,10 +9253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF46F0BE-CA28-4568-AEEA-82D636B2E98E}">
-  <dimension ref="A1:W106"/>
+  <dimension ref="A1:W104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9325,144 +9282,138 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="4">
         <v>44749</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44749</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+    <row r="4" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
         <v>44749</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6">
-        <v>17.372879999999999</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3" s="6" t="s">
+      <c r="D4" s="5">
+        <v>0.45277777777777778</v>
+      </c>
+      <c r="E4" s="3">
+        <v>238.81360000000001</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7">
-        <v>44749</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.45277777777777778</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="L4" s="3">
+        <f>MIN(E2:E10)</f>
         <v>238.81360000000001</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="6">
-        <f>MIN(E2:E10)</f>
-        <v>17.372879999999999</v>
-      </c>
-      <c r="M4" s="6">
+      <c r="M4" s="3">
         <f>MIN(E11:E19)</f>
         <v>224.2373</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="3">
         <f>MIN(E20:E28)</f>
         <v>263.22030000000001</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="3">
         <f>MIN(E29:E37)</f>
         <v>248.88140000000001</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="3">
         <f>MIN(E38:E44)</f>
         <v>459.22030000000001</v>
       </c>
-      <c r="Q4" s="6">
-        <f>MIN(E45:E53)</f>
+      <c r="Q4" s="3">
+        <f>MIN(E45:E51)</f>
         <v>393.11860000000001</v>
       </c>
-      <c r="R4" s="6">
-        <f>MIN(E54:E62)</f>
+      <c r="R4" s="3">
+        <f>MIN(E52:E60)</f>
         <v>452.10169999999999</v>
       </c>
-      <c r="S4" s="6">
-        <f>MIN(E63:E71)</f>
+      <c r="S4" s="3">
+        <f>MIN(E61:E69)</f>
         <v>3354.39</v>
       </c>
-      <c r="T4" s="6">
-        <f>MIN(E72:E76)</f>
+      <c r="T4" s="3">
+        <f>MIN(E70:E74)</f>
         <v>3202.6950000000002</v>
       </c>
-      <c r="U4" s="6">
-        <f>MIN(E77:E85)</f>
+      <c r="U4" s="3">
+        <f>MIN(E75:E83)</f>
         <v>1238.9490000000001</v>
       </c>
-      <c r="V4" s="6">
-        <f>MIN(E86:E88)</f>
+      <c r="V4" s="3">
+        <f>MIN(E84:E86)</f>
         <v>271.01690000000002</v>
       </c>
-      <c r="W4" s="6">
-        <f>MIN(E89:E97)</f>
+      <c r="W4" s="3">
+        <f>MIN(E87:E95)</f>
         <v>834.79629999999997</v>
       </c>
     </row>
@@ -9483,11 +9434,11 @@
         <v>376.87029999999999</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L5">
         <f>_xlfn.QUARTILE.INC(E2:E10,1)</f>
-        <v>305.72882500000003</v>
+        <v>335.74575000000004</v>
       </c>
       <c r="M5">
         <f>_xlfn.QUARTILE.INC(E11:E19,1)</f>
@@ -9506,31 +9457,31 @@
         <v>655.74575000000004</v>
       </c>
       <c r="Q5">
-        <f>_xlfn.QUARTILE.INC(E45:E53,1)</f>
-        <v>393.5847</v>
+        <f>_xlfn.QUARTILE.INC(E45:E51,1)</f>
+        <v>393.81774999999999</v>
       </c>
       <c r="R5">
-        <f>_xlfn.QUARTILE.INC(E54:E62,1)</f>
+        <f>_xlfn.QUARTILE.INC(E52:E60,1)</f>
         <v>452.14404999999999</v>
       </c>
       <c r="S5">
-        <f>_xlfn.QUARTILE.INC(E63:E71,1)</f>
+        <f>_xlfn.QUARTILE.INC(E61:E69,1)</f>
         <v>5026.1189999999997</v>
       </c>
       <c r="T5">
-        <f>_xlfn.QUARTILE.INC(E72:E76,1)</f>
+        <f>_xlfn.QUARTILE.INC(E70:E74,1)</f>
         <v>3431.8432499999999</v>
       </c>
       <c r="U5">
-        <f>_xlfn.QUARTILE.INC(E77:E85,1)</f>
+        <f>_xlfn.QUARTILE.INC(E75:E83,1)</f>
         <v>1568.508</v>
       </c>
       <c r="V5">
-        <f>_xlfn.QUARTILE.INC(E86:E88,1)</f>
+        <f>_xlfn.QUARTILE.INC(E84:E86,1)</f>
         <v>362.322</v>
       </c>
       <c r="W5">
-        <f>_xlfn.QUARTILE.INC(E89:E97,1)</f>
+        <f>_xlfn.QUARTILE.INC(E87:E95,1)</f>
         <v>1131.7460000000001</v>
       </c>
     </row>
@@ -9551,11 +9502,11 @@
         <v>343.45760000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L6">
         <f>_xlfn.QUARTILE.INC(E2:E10,2)</f>
-        <v>360.16395</v>
+        <v>376.87029999999999</v>
       </c>
       <c r="M6">
         <f>_xlfn.QUARTILE.INC(E11:E19,2)</f>
@@ -9574,31 +9525,31 @@
         <v>681.66629999999998</v>
       </c>
       <c r="Q6">
-        <f>_xlfn.QUARTILE.INC(E45:E53,2)</f>
-        <v>394.05079999999998</v>
+        <f>_xlfn.QUARTILE.INC(E45:E51,2)</f>
+        <v>412.39829999999995</v>
       </c>
       <c r="R6">
-        <f>_xlfn.QUARTILE.INC(E54:E62,2)</f>
+        <f>_xlfn.QUARTILE.INC(E52:E60,2)</f>
         <v>452.18639999999999</v>
       </c>
       <c r="S6">
-        <f>_xlfn.QUARTILE.INC(E63:E71,2)</f>
+        <f>_xlfn.QUARTILE.INC(E61:E69,2)</f>
         <v>6369.29</v>
       </c>
       <c r="T6">
-        <f>_xlfn.QUARTILE.INC(E72:E76,2)</f>
+        <f>_xlfn.QUARTILE.INC(E70:E74,2)</f>
         <v>3660.9915000000001</v>
       </c>
       <c r="U6">
-        <f>_xlfn.QUARTILE.INC(E77:E85,2)</f>
+        <f>_xlfn.QUARTILE.INC(E75:E83,2)</f>
         <v>2052.39</v>
       </c>
       <c r="V6">
-        <f>_xlfn.QUARTILE.INC(E86:E88,2)</f>
+        <f>_xlfn.QUARTILE.INC(E84:E86,2)</f>
         <v>453.62709999999998</v>
       </c>
       <c r="W6">
-        <f>_xlfn.QUARTILE.INC(E89:E97,2)</f>
+        <f>_xlfn.QUARTILE.INC(E87:E95,2)</f>
         <v>1407.2370000000001</v>
       </c>
     </row>
@@ -9619,11 +9570,11 @@
         <v>328.03390000000002</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L7">
         <f>_xlfn.QUARTILE.INC(E2:E10,3)</f>
-        <v>381.57627500000001</v>
+        <v>381.81354999999996</v>
       </c>
       <c r="M7">
         <f>_xlfn.QUARTILE.INC(E11:E19,3)</f>
@@ -9642,31 +9593,31 @@
         <v>725.51029999999992</v>
       </c>
       <c r="Q7">
-        <f>_xlfn.QUARTILE.INC(E45:E53,3)</f>
-        <v>414.47455000000002</v>
+        <f>_xlfn.QUARTILE.INC(E45:E51,3)</f>
+        <v>431.78392499999995</v>
       </c>
       <c r="R7">
-        <f>_xlfn.QUARTILE.INC(E54:E62,3)</f>
+        <f>_xlfn.QUARTILE.INC(E52:E60,3)</f>
         <v>471.67795000000001</v>
       </c>
       <c r="S7">
-        <f>_xlfn.QUARTILE.INC(E63:E71,3)</f>
+        <f>_xlfn.QUARTILE.INC(E61:E69,3)</f>
         <v>7530.3050000000003</v>
       </c>
       <c r="T7">
-        <f>_xlfn.QUARTILE.INC(E72:E76,3)</f>
+        <f>_xlfn.QUARTILE.INC(E70:E74,3)</f>
         <v>3890.1397499999998</v>
       </c>
       <c r="U7">
-        <f>_xlfn.QUARTILE.INC(E77:E85,3)</f>
+        <f>_xlfn.QUARTILE.INC(E75:E83,3)</f>
         <v>2633.4749999999999</v>
       </c>
       <c r="V7">
-        <f>_xlfn.QUARTILE.INC(E86:E88,3)</f>
+        <f>_xlfn.QUARTILE.INC(E84:E86,3)</f>
         <v>455.06780000000003</v>
       </c>
       <c r="W7">
-        <f>_xlfn.QUARTILE.INC(E89:E97,3)</f>
+        <f>_xlfn.QUARTILE.INC(E87:E95,3)</f>
         <v>1459.441</v>
       </c>
     </row>
@@ -9687,7 +9638,7 @@
         <v>461.84750000000003</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L8">
         <f>MAX(E2:E10)</f>
@@ -9710,31 +9661,31 @@
         <v>843.44069999999999</v>
       </c>
       <c r="Q8">
-        <f>MAX(E45:E53)</f>
+        <f>MAX(E45:E51)</f>
         <v>434.89830000000001</v>
       </c>
       <c r="R8">
-        <f>MAX(E54:E62)</f>
+        <f>MAX(E52:E60)</f>
         <v>491.16950000000003</v>
       </c>
       <c r="S8">
-        <f>MAX(E63:E71)</f>
+        <f>MAX(E61:E69)</f>
         <v>10517.98</v>
       </c>
       <c r="T8">
-        <f>MAX(E72:E76)</f>
+        <f>MAX(E70:E74)</f>
         <v>4119.2879999999996</v>
       </c>
       <c r="U8">
-        <f>MAX(E77:E85)</f>
+        <f>MAX(E75:E83)</f>
         <v>2769.0680000000002</v>
       </c>
       <c r="V8">
-        <f>MAX(E86:E88)</f>
+        <f>MAX(E84:E86)</f>
         <v>456.50850000000003</v>
       </c>
       <c r="W8">
-        <f>MAX(E89:E97)</f>
+        <f>MAX(E87:E95)</f>
         <v>1625.712</v>
       </c>
     </row>
@@ -9772,11 +9723,11 @@
         <v>382.28809999999999</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L10">
         <f>AVERAGE(E2:E10)</f>
-        <v>316.25286000000006</v>
+        <v>358.9500000000001</v>
       </c>
       <c r="M10">
         <f>AVERAGE(E11:E19)</f>
@@ -9795,131 +9746,131 @@
         <v>678.11991428571423</v>
       </c>
       <c r="Q10">
-        <f>AVERAGE(E45:E53)</f>
-        <v>407.35590000000002</v>
+        <f>AVERAGE(E45:E51)</f>
+        <v>413.20337499999999</v>
       </c>
       <c r="R10">
-        <f>AVERAGE(E54:E62)</f>
+        <f>AVERAGE(E52:E60)</f>
         <v>465.15253333333334</v>
       </c>
       <c r="S10">
-        <f>AVERAGE(E63:E71)</f>
+        <f>AVERAGE(E61:E69)</f>
         <v>6582.6496666666671</v>
       </c>
       <c r="T10">
-        <f>AVERAGE(E72:E76)</f>
+        <f>AVERAGE(E70:E74)</f>
         <v>3660.9915000000001</v>
       </c>
       <c r="U10">
-        <f>AVERAGE(E77:E85)</f>
+        <f>AVERAGE(E75:E83)</f>
         <v>2044.2975555555556</v>
       </c>
       <c r="V10">
-        <f>AVERAGE(E86:E88)</f>
+        <f>AVERAGE(E84:E86)</f>
         <v>393.71750000000003</v>
       </c>
       <c r="W10">
-        <f>AVERAGE(E89:E97)</f>
+        <f>AVERAGE(E87:E95)</f>
         <v>1290.1205888888887</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+    <row r="11" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <v>44749</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="5">
         <v>0.50902777777777775</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="3">
         <v>227.20339999999999</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="K11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="3">
         <f>L8-L4</f>
-        <v>444.47462000000002</v>
-      </c>
-      <c r="M11" s="6">
+        <v>223.03390000000002</v>
+      </c>
+      <c r="M11" s="3">
         <f t="shared" ref="M11:W11" si="0">M8-M4</f>
         <v>117.77960000000002</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="3">
         <f t="shared" si="0"/>
         <v>275.334</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="3">
         <f t="shared" si="0"/>
         <v>415.84739999999999</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="3">
         <f t="shared" si="0"/>
         <v>384.22039999999998</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="3">
         <f t="shared" si="0"/>
         <v>41.779699999999991</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="3">
         <f t="shared" si="0"/>
         <v>39.067800000000034</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="3">
         <f t="shared" si="0"/>
         <v>7163.59</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="3">
         <f t="shared" si="0"/>
         <v>916.59299999999939</v>
       </c>
-      <c r="U11" s="6">
+      <c r="U11" s="3">
         <f t="shared" si="0"/>
         <v>1530.1190000000001</v>
       </c>
-      <c r="V11" s="6">
+      <c r="V11" s="3">
         <f t="shared" si="0"/>
         <v>185.49160000000001</v>
       </c>
-      <c r="W11" s="6">
+      <c r="W11" s="3">
         <f t="shared" si="0"/>
         <v>790.91570000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
+    <row r="12" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>44749</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="5">
         <v>0.51874999999999993</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="3">
         <v>224.2373</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
+    <row r="13" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
         <v>2</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="4">
         <v>44749</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -10024,43 +9975,43 @@
         <v>292.18639999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>44749</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="F20" s="6" t="s">
-        <v>14</v>
+      <c r="D20" s="5"/>
+      <c r="E20" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>44749</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="5">
         <v>0.55972222222222223</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>263.22030000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="4">
         <v>44749</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="5">
         <v>0.56458333333333333</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>275.50850000000003</v>
       </c>
     </row>
@@ -10178,7 +10129,7 @@
       </c>
       <c r="D29" s="12"/>
       <c r="F29" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -10193,7 +10144,7 @@
       </c>
       <c r="D30" s="12"/>
       <c r="F30" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -10445,7 +10396,7 @@
         <v>44742</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -10459,7 +10410,7 @@
         <v>44742</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -10473,49 +10424,58 @@
         <v>44742</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="8">
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
         <v>6</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="3">
         <v>1</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="4">
         <v>44753</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>14</v>
+      <c r="D48" s="5">
+        <v>0.57361111111111118</v>
+      </c>
+      <c r="E48" s="3">
+        <v>430.74579999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="8">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
         <v>6</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="E49">
+        <v>394.05079999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50">
         <v>2</v>
       </c>
-      <c r="C49" s="9">
-        <v>44753</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="8">
-        <v>6</v>
-      </c>
-      <c r="B50" s="8">
-        <v>3</v>
-      </c>
-      <c r="C50" s="9">
-        <v>44753</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>14</v>
+      <c r="C50" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="E50">
+        <v>434.89830000000001</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -10523,50 +10483,44 @@
         <v>6</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C51" s="1">
         <v>44761</v>
       </c>
       <c r="D51" s="2">
-        <v>0.52916666666666667</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="E51">
-        <v>394.05079999999998</v>
+        <v>393.11860000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>6</v>
-      </c>
-      <c r="B52">
+    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6">
+        <v>7</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" s="7">
+        <v>44742</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6">
+        <v>7</v>
+      </c>
+      <c r="B53" s="6">
         <v>2</v>
       </c>
-      <c r="C52" s="1">
-        <v>44761</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0.53680555555555554</v>
-      </c>
-      <c r="E52">
-        <v>434.89830000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>6</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-      <c r="C53" s="1">
-        <v>44761</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0.54999999999999993</v>
-      </c>
-      <c r="E53">
-        <v>393.11860000000001</v>
+      <c r="C53" s="7">
+        <v>44742</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -10574,41 +10528,41 @@
         <v>7</v>
       </c>
       <c r="B54" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C54" s="7">
         <v>44742</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6">
+    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="8">
         <v>7</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="8">
+        <v>1</v>
+      </c>
+      <c r="C55" s="9">
+        <v>44753</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="8">
+        <v>7</v>
+      </c>
+      <c r="B56" s="8">
         <v>2</v>
       </c>
-      <c r="C55" s="7">
-        <v>44742</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6">
-        <v>7</v>
-      </c>
-      <c r="B56" s="6">
-        <v>3</v>
-      </c>
-      <c r="C56" s="7">
-        <v>44742</v>
+      <c r="C56" s="9">
+        <v>44753</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -10616,41 +10570,47 @@
         <v>7</v>
       </c>
       <c r="B57" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C57" s="9">
         <v>44753</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="8">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
         <v>7</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="E58">
+        <v>452.10169999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>7</v>
+      </c>
+      <c r="B59">
         <v>2</v>
       </c>
-      <c r="C58" s="9">
-        <v>44753</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="8">
-        <v>7</v>
-      </c>
-      <c r="B59" s="8">
-        <v>3</v>
-      </c>
-      <c r="C59" s="9">
-        <v>44753</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>14</v>
+      <c r="C59" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="E59">
+        <v>491.16950000000003</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -10658,50 +10618,50 @@
         <v>7</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C60" s="1">
         <v>44761</v>
       </c>
       <c r="D60" s="2">
-        <v>0.49027777777777781</v>
+        <v>0.5083333333333333</v>
       </c>
       <c r="E60">
-        <v>452.10169999999999</v>
+        <v>452.18639999999999</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>7</v>
-      </c>
-      <c r="B61">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1</v>
       </c>
       <c r="C61" s="1">
-        <v>44761</v>
+        <v>44747</v>
       </c>
       <c r="D61" s="2">
-        <v>0.50069444444444444</v>
+        <v>0.41111111111111115</v>
       </c>
       <c r="E61">
-        <v>491.16950000000003</v>
+        <v>9397.9320000000007</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>7</v>
-      </c>
-      <c r="B62">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B62" s="3">
+        <v>2</v>
       </c>
       <c r="C62" s="1">
-        <v>44761</v>
+        <v>44747</v>
       </c>
       <c r="D62" s="2">
-        <v>0.5083333333333333</v>
+        <v>0.42222222222222222</v>
       </c>
       <c r="E62">
-        <v>452.18639999999999</v>
+        <v>7530.3050000000003</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -10709,50 +10669,50 @@
         <v>8</v>
       </c>
       <c r="B63" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C63" s="1">
         <v>44747</v>
       </c>
       <c r="D63" s="2">
-        <v>0.41111111111111115</v>
+        <v>0.42986111111111108</v>
       </c>
       <c r="E63">
-        <v>9397.9320000000007</v>
+        <v>3354.39</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
-      <c r="B64" s="3">
-        <v>2</v>
+      <c r="B64">
+        <v>1</v>
       </c>
       <c r="C64" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D64" s="2">
-        <v>0.42222222222222222</v>
+        <v>0.42638888888888887</v>
       </c>
       <c r="E64">
-        <v>7530.3050000000003</v>
+        <v>10517.98</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
-      <c r="B65" s="3">
-        <v>3</v>
+      <c r="B65">
+        <v>2</v>
       </c>
       <c r="C65" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D65" s="2">
-        <v>0.42986111111111108</v>
+        <v>0.4375</v>
       </c>
       <c r="E65">
-        <v>3354.39</v>
+        <v>7493.1189999999997</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -10760,16 +10720,16 @@
         <v>8</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" s="1">
         <v>44750</v>
       </c>
       <c r="D66" s="2">
-        <v>0.42638888888888887</v>
+        <v>0.44513888888888892</v>
       </c>
       <c r="E66">
-        <v>10517.98</v>
+        <v>6369.29</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -10777,16 +10737,16 @@
         <v>8</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D67" s="2">
-        <v>0.4375</v>
+        <v>0.42777777777777781</v>
       </c>
       <c r="E67">
-        <v>7493.1189999999997</v>
+        <v>5026.1189999999997</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -10794,16 +10754,16 @@
         <v>8</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D68" s="2">
-        <v>0.44513888888888892</v>
+        <v>0.43541666666666662</v>
       </c>
       <c r="E68">
-        <v>6369.29</v>
+        <v>5242.5590000000002</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -10811,67 +10771,58 @@
         <v>8</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69" s="1">
         <v>44760</v>
       </c>
       <c r="D69" s="2">
-        <v>0.42777777777777781</v>
+        <v>0.4458333333333333</v>
       </c>
       <c r="E69">
-        <v>5026.1189999999997</v>
+        <v>4312.1530000000002</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1">
+        <v>44747</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.46111111111111108</v>
+      </c>
+      <c r="E70">
+        <v>4119.2879999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="10">
+        <v>9</v>
+      </c>
+      <c r="B71" s="10">
+        <v>1</v>
+      </c>
+      <c r="C71" s="11">
+        <v>44750</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="10">
+        <v>9</v>
+      </c>
+      <c r="B72" s="10">
         <v>2</v>
       </c>
-      <c r="C70" s="1">
-        <v>44760</v>
-      </c>
-      <c r="D70" s="2">
-        <v>0.43541666666666662</v>
-      </c>
-      <c r="E70">
-        <v>5242.5590000000002</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>8</v>
-      </c>
-      <c r="B71">
-        <v>3</v>
-      </c>
-      <c r="C71" s="1">
-        <v>44760</v>
-      </c>
-      <c r="D71" s="2">
-        <v>0.4458333333333333</v>
-      </c>
-      <c r="E71">
-        <v>4312.1530000000002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>9</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" s="1">
-        <v>44747</v>
-      </c>
-      <c r="D72" s="2">
-        <v>0.46111111111111108</v>
-      </c>
-      <c r="E72">
-        <v>4119.2879999999996</v>
+      <c r="C72" s="11">
+        <v>44750</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -10879,52 +10830,61 @@
         <v>9</v>
       </c>
       <c r="B73" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C73" s="11">
         <v>44750</v>
       </c>
-      <c r="G73" s="10" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="74" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="10">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74">
         <v>9</v>
       </c>
-      <c r="B74" s="10">
-        <v>2</v>
-      </c>
-      <c r="C74" s="11">
-        <v>44750</v>
+      <c r="B74" s="3">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>44760</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="E74">
+        <v>3202.6950000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="10">
-        <v>9</v>
-      </c>
-      <c r="B75" s="10">
-        <v>3</v>
-      </c>
-      <c r="C75" s="11">
-        <v>44750</v>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1">
+        <v>44747</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="E75">
+        <v>1238.9490000000001</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>9</v>
-      </c>
-      <c r="B76" s="3">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
       </c>
       <c r="C76" s="1">
-        <v>44760</v>
+        <v>44747</v>
       </c>
       <c r="D76" s="2">
-        <v>0.41250000000000003</v>
+        <v>0.4916666666666667</v>
       </c>
       <c r="E76">
-        <v>3202.6950000000002</v>
+        <v>1888.932</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -10932,16 +10892,16 @@
         <v>10</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1">
         <v>44747</v>
       </c>
       <c r="D77" s="2">
-        <v>0.48055555555555557</v>
+        <v>0.5</v>
       </c>
       <c r="E77">
-        <v>1238.9490000000001</v>
+        <v>2716.78</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -10949,16 +10909,16 @@
         <v>10</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D78" s="2">
-        <v>0.4916666666666667</v>
+        <v>0.49236111111111108</v>
       </c>
       <c r="E78">
-        <v>1888.932</v>
+        <v>1371.4069999999999</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -10966,16 +10926,16 @@
         <v>10</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D79" s="2">
-        <v>0.5</v>
+        <v>0.50069444444444444</v>
       </c>
       <c r="E79">
-        <v>2716.78</v>
+        <v>2052.39</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -10983,50 +10943,50 @@
         <v>10</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C80" s="1">
         <v>44750</v>
       </c>
       <c r="D80" s="2">
-        <v>0.49236111111111108</v>
+        <v>0.50624999999999998</v>
       </c>
       <c r="E80">
-        <v>1371.4069999999999</v>
+        <v>2159.1689999999999</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>10</v>
       </c>
-      <c r="B81">
-        <v>2</v>
+      <c r="B81" s="3">
+        <v>1</v>
       </c>
       <c r="C81" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D81" s="2">
-        <v>0.50069444444444444</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="E81">
-        <v>2052.39</v>
+        <v>1568.508</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>10</v>
       </c>
-      <c r="B82">
-        <v>3</v>
+      <c r="B82" s="3">
+        <v>2</v>
       </c>
       <c r="C82" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D82" s="2">
-        <v>0.50624999999999998</v>
+        <v>0.4694444444444445</v>
       </c>
       <c r="E82">
-        <v>2159.1689999999999</v>
+        <v>2633.4749999999999</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -11034,152 +10994,152 @@
         <v>10</v>
       </c>
       <c r="B83" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C83" s="1">
         <v>44760</v>
       </c>
       <c r="D83" s="2">
-        <v>0.4597222222222222</v>
+        <v>0.4777777777777778</v>
       </c>
       <c r="E83">
-        <v>1568.508</v>
+        <v>2769.0680000000002</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B84" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" s="1">
-        <v>44760</v>
+        <v>44753</v>
       </c>
       <c r="D84" s="2">
-        <v>0.4694444444444445</v>
+        <v>0.47083333333333338</v>
       </c>
       <c r="E84">
-        <v>2633.4749999999999</v>
+        <v>271.01690000000002</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>10</v>
-      </c>
-      <c r="B85" s="3">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
       </c>
       <c r="C85" s="1">
-        <v>44760</v>
+        <v>44761</v>
       </c>
       <c r="D85" s="2">
-        <v>0.4777777777777778</v>
+        <v>0.50763888888888886</v>
       </c>
       <c r="E85">
-        <v>2769.0680000000002</v>
+        <v>453.62709999999998</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>11</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86">
         <v>1</v>
       </c>
       <c r="C86" s="1">
-        <v>44753</v>
+        <v>44764</v>
       </c>
       <c r="D86" s="2">
-        <v>0.47083333333333338</v>
+        <v>0.51597222222222217</v>
       </c>
       <c r="E86">
-        <v>271.01690000000002</v>
+        <v>456.50850000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>11</v>
-      </c>
-      <c r="B87">
+    <row r="87" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="3">
+        <v>12</v>
+      </c>
+      <c r="B87" s="3">
         <v>1</v>
       </c>
-      <c r="C87" s="1">
-        <v>44761</v>
-      </c>
-      <c r="D87" s="2">
-        <v>0.50763888888888886</v>
-      </c>
-      <c r="E87">
-        <v>453.62709999999998</v>
+      <c r="C87" s="4">
+        <v>44748</v>
+      </c>
+      <c r="D87" s="5">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="E87" s="3">
+        <v>1154.627</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>11</v>
-      </c>
-      <c r="B88">
+    <row r="88" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="3">
+        <v>12</v>
+      </c>
+      <c r="B88" s="3">
+        <v>2</v>
+      </c>
+      <c r="C88" s="4">
+        <v>44748</v>
+      </c>
+      <c r="D88" s="5">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="E88" s="3">
+        <v>1131.7460000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="3">
+        <v>12</v>
+      </c>
+      <c r="B89" s="3">
+        <v>3</v>
+      </c>
+      <c r="C89" s="4">
+        <v>44748</v>
+      </c>
+      <c r="D89" s="5">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="E89" s="3">
+        <v>1113.78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>12</v>
+      </c>
+      <c r="B90" s="3">
         <v>1</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C90" s="1">
         <v>44764</v>
       </c>
-      <c r="D88" s="2">
-        <v>0.51597222222222217</v>
-      </c>
-      <c r="E88">
-        <v>456.50850000000003</v>
+      <c r="D90" s="2">
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="E90">
+        <v>834.79629999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="6">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91">
         <v>12</v>
       </c>
-      <c r="B89" s="6">
-        <v>1</v>
-      </c>
-      <c r="C89" s="7">
-        <v>44748</v>
-      </c>
-      <c r="D89" s="12">
-        <v>0.5180555555555556</v>
-      </c>
-      <c r="E89" s="6">
-        <v>1154.627</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="6">
-        <v>12</v>
-      </c>
-      <c r="B90" s="6">
+      <c r="B91" s="3">
         <v>2</v>
       </c>
-      <c r="C90" s="7">
-        <v>44748</v>
-      </c>
-      <c r="D90" s="12">
-        <v>0.53194444444444444</v>
-      </c>
-      <c r="E90" s="6">
-        <v>1131.7460000000001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="6">
-        <v>12</v>
-      </c>
-      <c r="B91" s="6">
-        <v>3</v>
-      </c>
-      <c r="C91" s="7">
-        <v>44748</v>
-      </c>
-      <c r="D91" s="12">
-        <v>0.54236111111111118</v>
-      </c>
-      <c r="E91" s="6">
-        <v>1113.78</v>
+      <c r="C91" s="1">
+        <v>44764</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="E91">
+        <v>1625.712</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
@@ -11187,16 +11147,16 @@
         <v>12</v>
       </c>
       <c r="B92" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C92" s="1">
         <v>44764</v>
       </c>
       <c r="D92" s="2">
-        <v>0.40138888888888885</v>
+        <v>0.42291666666666666</v>
       </c>
       <c r="E92">
-        <v>834.79629999999997</v>
+        <v>1475.712</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
@@ -11204,16 +11164,16 @@
         <v>12</v>
       </c>
       <c r="B93" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93" s="1">
-        <v>44764</v>
+        <v>44769</v>
       </c>
       <c r="D93" s="2">
-        <v>0.41250000000000003</v>
+        <v>0.40416666666666662</v>
       </c>
       <c r="E93">
-        <v>1625.712</v>
+        <v>1459.441</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
@@ -11221,16 +11181,16 @@
         <v>12</v>
       </c>
       <c r="B94" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" s="1">
-        <v>44764</v>
+        <v>44769</v>
       </c>
       <c r="D94" s="2">
-        <v>0.42291666666666666</v>
+        <v>0.41944444444444445</v>
       </c>
       <c r="E94">
-        <v>1475.712</v>
+        <v>1407.2370000000001</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -11238,60 +11198,26 @@
         <v>12</v>
       </c>
       <c r="B95" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C95" s="1">
         <v>44769</v>
       </c>
       <c r="D95" s="2">
-        <v>0.40416666666666662</v>
+        <v>0.4291666666666667</v>
       </c>
       <c r="E95">
-        <v>1459.441</v>
+        <v>1408.0340000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>12</v>
-      </c>
-      <c r="B96" s="3">
-        <v>2</v>
-      </c>
-      <c r="C96" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D96" s="2">
-        <v>0.41944444444444445</v>
-      </c>
-      <c r="E96">
-        <v>1407.2370000000001</v>
-      </c>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B102" s="3"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>12</v>
-      </c>
-      <c r="B97" s="3">
-        <v>3</v>
-      </c>
-      <c r="C97" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D97" s="2">
-        <v>0.4291666666666667</v>
-      </c>
-      <c r="E97">
-        <v>1408.0340000000001</v>
-      </c>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B103" s="3"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B106" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11303,8 +11229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1A6D3F-3AEF-49D2-BA63-6C5B3E7AF95E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W20" workbookViewId="0">
-      <selection activeCell="AE23" sqref="AE23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated data for wetland data
</commit_message>
<xml_diff>
--- a/Wetlands/Wetland data.xlsx
+++ b/Wetlands/Wetland data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymad138\Documents\Ecuador2022\Wetlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49C0982-E0C4-493B-9B56-FDEC2BEE7E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA1DD22-3CAC-4A2C-BD44-2537DF0EB828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="6280" xr2:uid="{94E7109B-EF61-4772-AC1F-D142A6519923}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Wetland</t>
   </si>
@@ -66,9 +66,6 @@
     <t>10:38-10:39</t>
   </si>
   <si>
-    <t>The plot is just flat and doesn’t look right</t>
-  </si>
-  <si>
     <t xml:space="preserve">Graphs do not show on this </t>
   </si>
   <si>
@@ -82,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +87,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,12 +104,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -132,9 +129,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF46F0BE-CA28-4568-AEEA-82D636B2E98E}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +492,7 @@
         <v>44749</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -511,7 +509,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -680,7 +678,7 @@
         <v>44749</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -794,7 +792,7 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -937,9 +935,9 @@
       <c r="C29" s="7">
         <v>44741</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="8"/>
       <c r="F29" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -952,9 +950,9 @@
       <c r="C30" s="7">
         <v>44741</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="8"/>
       <c r="F30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -967,7 +965,7 @@
       <c r="C31" s="7">
         <v>44741</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="8">
         <v>0.4284722222222222</v>
       </c>
       <c r="E31" s="6">
@@ -1206,7 +1204,7 @@
         <v>44742</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1220,7 +1218,7 @@
         <v>44742</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1234,7 +1232,7 @@
         <v>44742</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1316,7 +1314,7 @@
         <v>44742</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1330,7 +1328,7 @@
         <v>44742</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1344,49 +1342,58 @@
         <v>44742</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="9">
         <v>7</v>
       </c>
-      <c r="B55" s="8">
-        <v>1</v>
-      </c>
-      <c r="C55" s="9">
+      <c r="B55" s="9">
+        <v>1</v>
+      </c>
+      <c r="C55" s="10">
         <v>44753</v>
       </c>
-      <c r="F55" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="8">
+      <c r="D55" s="11">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E55" s="9">
+        <v>268.98309999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="9">
         <v>7</v>
       </c>
-      <c r="B56" s="8">
-        <v>2</v>
-      </c>
-      <c r="C56" s="9">
+      <c r="B56" s="9">
+        <v>2</v>
+      </c>
+      <c r="C56" s="10">
         <v>44753</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="8">
+      <c r="D56" s="11">
+        <v>0.52013888888888882</v>
+      </c>
+      <c r="E56" s="9">
+        <v>225.1695</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="9">
         <v>7</v>
       </c>
-      <c r="B57" s="8">
-        <v>3</v>
-      </c>
-      <c r="C57" s="9">
+      <c r="B57" s="9">
+        <v>3</v>
+      </c>
+      <c r="C57" s="10">
         <v>44753</v>
       </c>
-      <c r="F57" s="6" t="s">
-        <v>13</v>
+      <c r="D57" s="11">
+        <v>0.53263888888888888</v>
+      </c>
+      <c r="E57" s="9">
+        <v>240.8475</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated data for ppm charts and all of the not corrected ppm is collected
</commit_message>
<xml_diff>
--- a/Wetlands/Wetland data.xlsx
+++ b/Wetlands/Wetland data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymad138\Documents\Ecuador2022\Wetlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FF606B-E017-4462-8DB1-955FAE28BDA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934483F-A98C-4320-BE27-377176A58A52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="6280" xr2:uid="{94E7109B-EF61-4772-AC1F-D142A6519923}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Wetland</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>10:38-10:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graphs do not show on this </t>
   </si>
   <si>
     <t>NA</t>
@@ -117,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -125,8 +122,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -449,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF46F0BE-CA28-4568-AEEA-82D636B2E98E}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -489,7 +484,7 @@
         <v>44749</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -506,7 +501,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -675,7 +670,7 @@
         <v>44749</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -729,7 +724,7 @@
         <v>342.01690000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -746,7 +741,7 @@
         <v>290.40679999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -763,7 +758,7 @@
         <v>330.9153</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -780,7 +775,7 @@
         <v>292.18639999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -789,10 +784,10 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -806,7 +801,7 @@
         <v>263.22030000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -820,7 +815,7 @@
         <v>275.50850000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3</v>
       </c>
@@ -837,7 +832,7 @@
         <v>342.91149999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3</v>
       </c>
@@ -854,7 +849,7 @@
         <v>401.7627</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3</v>
       </c>
@@ -871,7 +866,7 @@
         <v>401.59320000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3</v>
       </c>
@@ -888,7 +883,7 @@
         <v>487.61020000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3</v>
       </c>
@@ -905,7 +900,7 @@
         <v>536.33900000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>3</v>
       </c>
@@ -922,586 +917,599 @@
         <v>538.55430000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
         <v>4</v>
       </c>
-      <c r="B29" s="6">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7">
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
         <v>44741</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
+      <c r="D29" s="5">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="E29" s="3">
+        <v>588.96609999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
         <v>4</v>
       </c>
-      <c r="B30" s="6">
-        <v>2</v>
-      </c>
-      <c r="C30" s="7">
-        <v>44741</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="F30" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4">
+        <v>44757</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.54027777777777775</v>
+      </c>
+      <c r="E30" s="3">
+        <v>593.62710000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
         <v>4</v>
       </c>
-      <c r="B31" s="6">
-        <v>3</v>
-      </c>
-      <c r="C31" s="7">
-        <v>44741</v>
-      </c>
-      <c r="D31" s="8">
-        <v>0.4284722222222222</v>
-      </c>
-      <c r="E31" s="6">
-        <v>248.88140000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4">
+        <v>44757</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E31" s="3">
+        <v>664.72879999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>4</v>
       </c>
       <c r="B32" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32" s="4">
         <v>44757</v>
       </c>
       <c r="D32" s="5">
-        <v>0.54027777777777775</v>
+        <v>0.55972222222222223</v>
       </c>
       <c r="E32" s="3">
-        <v>593.62710000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
+        <v>653.79660000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>4</v>
       </c>
-      <c r="B33" s="3">
-        <v>2</v>
-      </c>
-      <c r="C33" s="4">
-        <v>44757</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0.54861111111111105</v>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>44764</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.4548611111111111</v>
       </c>
       <c r="E33" s="3">
-        <v>664.72879999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+        <v>395.83049999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>4</v>
       </c>
-      <c r="B34" s="3">
-        <v>3</v>
-      </c>
-      <c r="C34" s="4">
-        <v>44757</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0.55972222222222223</v>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>44764</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.46666666666666662</v>
       </c>
       <c r="E34" s="3">
-        <v>653.79660000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+        <v>492.61020000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1">
         <v>44764</v>
       </c>
       <c r="D35" s="2">
-        <v>0.4548611111111111</v>
+        <v>0.47083333333333338</v>
       </c>
       <c r="E35" s="3">
-        <v>395.83049999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+        <v>492.35590000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="1">
-        <v>44764</v>
+        <v>44740</v>
       </c>
       <c r="D36" s="2">
-        <v>0.46666666666666662</v>
+        <v>0.44305555555555554</v>
       </c>
       <c r="E36" s="3">
-        <v>492.61020000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+        <v>756.20699999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" s="1">
-        <v>44764</v>
+        <v>44740</v>
       </c>
       <c r="D37" s="2">
-        <v>0.47083333333333338</v>
+        <v>0.45763888888888887</v>
       </c>
       <c r="E37" s="3">
-        <v>492.35590000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+        <v>681.66629999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1">
         <v>44740</v>
       </c>
       <c r="D38" s="2">
-        <v>0.44305555555555554</v>
+        <v>0.47638888888888892</v>
       </c>
       <c r="E38" s="3">
-        <v>756.20699999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+        <v>669.47460000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>44740</v>
+        <v>44761</v>
       </c>
       <c r="D39" s="2">
-        <v>0.45763888888888887</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="E39" s="3">
-        <v>681.66629999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+        <v>459.22030000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>44740</v>
+        <v>44769</v>
       </c>
       <c r="D40" s="2">
-        <v>0.47638888888888892</v>
+        <v>0.47361111111111115</v>
       </c>
       <c r="E40" s="3">
-        <v>669.47460000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+        <v>843.44069999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="1">
-        <v>44761</v>
+        <v>44769</v>
       </c>
       <c r="D41" s="2">
-        <v>0.42708333333333331</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="E41" s="3">
-        <v>459.22030000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+        <v>694.81359999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42" s="1">
         <v>44769</v>
       </c>
       <c r="D42" s="2">
-        <v>0.47361111111111115</v>
+        <v>0.49652777777777773</v>
       </c>
       <c r="E42" s="3">
-        <v>843.44069999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>5</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D43" s="2">
-        <v>0.48749999999999999</v>
+        <v>642.01689999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>44742</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0.51041666666666663</v>
       </c>
       <c r="E43" s="3">
-        <v>694.81359999999995</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D44" s="2">
-        <v>0.49652777777777773</v>
+        <v>442.44069999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>6</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4">
+        <v>44753</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0.57361111111111118</v>
       </c>
       <c r="E44" s="3">
-        <v>642.01689999999996</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
+        <v>430.74579999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45">
         <v>6</v>
       </c>
-      <c r="B45" s="6">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="E45">
+        <v>394.05079999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="E46">
+        <v>434.89830000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44761</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="E47">
+        <v>393.11860000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>7</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4">
         <v>44742</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="6">
-        <v>6</v>
-      </c>
-      <c r="B46" s="6">
-        <v>2</v>
-      </c>
-      <c r="C46" s="7">
+      <c r="D48" s="5">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="E48" s="3">
+        <v>728.71190000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>7</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4">
         <v>44742</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6">
-        <v>6</v>
-      </c>
-      <c r="B47" s="6">
-        <v>3</v>
-      </c>
-      <c r="C47" s="7">
+      <c r="D49" s="5">
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="E49" s="3">
+        <v>779.38980000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>7</v>
+      </c>
+      <c r="B50" s="3">
+        <v>3</v>
+      </c>
+      <c r="C50" s="4">
         <v>44742</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="3">
-        <v>6</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-      <c r="C48" s="4">
+      <c r="D50" s="5">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E50" s="3">
+        <v>253.81360000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7">
+        <v>7</v>
+      </c>
+      <c r="B51" s="7">
+        <v>1</v>
+      </c>
+      <c r="C51" s="8">
         <v>44753</v>
       </c>
-      <c r="D48" s="5">
-        <v>0.57361111111111118</v>
-      </c>
-      <c r="E48" s="3">
-        <v>430.74579999999997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>6</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1">
+      <c r="D51" s="9">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E51" s="7">
+        <v>268.98309999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7">
+        <v>7</v>
+      </c>
+      <c r="B52" s="7">
+        <v>2</v>
+      </c>
+      <c r="C52" s="8">
+        <v>44753</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0.52013888888888882</v>
+      </c>
+      <c r="E52" s="7">
+        <v>225.1695</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7">
+        <v>7</v>
+      </c>
+      <c r="B53" s="7">
+        <v>3</v>
+      </c>
+      <c r="C53" s="8">
+        <v>44753</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0.53263888888888888</v>
+      </c>
+      <c r="E53" s="7">
+        <v>240.8475</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
         <v>44761</v>
       </c>
-      <c r="D49" s="2">
-        <v>0.52916666666666667</v>
-      </c>
-      <c r="E49">
-        <v>394.05079999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>6</v>
-      </c>
-      <c r="B50">
-        <v>2</v>
-      </c>
-      <c r="C50" s="1">
+      <c r="D54" s="2">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="E54">
+        <v>452.10169999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1">
         <v>44761</v>
       </c>
-      <c r="D50" s="2">
-        <v>0.53680555555555554</v>
-      </c>
-      <c r="E50">
-        <v>434.89830000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>6</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51" s="1">
+      <c r="D55" s="2">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="E55">
+        <v>491.16950000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>7</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1">
         <v>44761</v>
       </c>
-      <c r="D51" s="2">
-        <v>0.54999999999999993</v>
-      </c>
-      <c r="E51">
-        <v>393.11860000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3">
-        <v>7</v>
-      </c>
-      <c r="B52" s="3">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4">
-        <v>44742</v>
-      </c>
-      <c r="D52" s="5">
-        <v>0.45624999999999999</v>
-      </c>
-      <c r="E52" s="3">
-        <v>728.71190000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3">
-        <v>7</v>
-      </c>
-      <c r="B53" s="3">
-        <v>2</v>
-      </c>
-      <c r="C53" s="4">
-        <v>44742</v>
-      </c>
-      <c r="D53" s="5">
-        <v>0.46666666666666662</v>
-      </c>
-      <c r="E53" s="3">
-        <v>779.38980000000004</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="3">
-        <v>7</v>
-      </c>
-      <c r="B54" s="3">
-        <v>3</v>
-      </c>
-      <c r="C54" s="4">
-        <v>44742</v>
-      </c>
-      <c r="D54" s="5">
-        <v>0.47569444444444442</v>
-      </c>
-      <c r="E54" s="3">
-        <v>253.81360000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="9">
-        <v>7</v>
-      </c>
-      <c r="B55" s="9">
-        <v>1</v>
-      </c>
-      <c r="C55" s="10">
-        <v>44753</v>
-      </c>
-      <c r="D55" s="11">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="E55" s="9">
-        <v>268.98309999999998</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="9">
-        <v>7</v>
-      </c>
-      <c r="B56" s="9">
-        <v>2</v>
-      </c>
-      <c r="C56" s="10">
-        <v>44753</v>
-      </c>
-      <c r="D56" s="11">
-        <v>0.52013888888888882</v>
-      </c>
-      <c r="E56" s="9">
-        <v>225.1695</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="9">
-        <v>7</v>
-      </c>
-      <c r="B57" s="9">
-        <v>3</v>
-      </c>
-      <c r="C57" s="10">
-        <v>44753</v>
-      </c>
-      <c r="D57" s="11">
-        <v>0.53263888888888888</v>
-      </c>
-      <c r="E57" s="9">
-        <v>240.8475</v>
+      <c r="D56" s="2">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="E56">
+        <v>452.18639999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>8</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>44747</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="E57">
+        <v>9397.9320000000007</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>7</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2</v>
       </c>
       <c r="C58" s="1">
-        <v>44761</v>
+        <v>44747</v>
       </c>
       <c r="D58" s="2">
-        <v>0.49027777777777781</v>
+        <v>0.42222222222222222</v>
       </c>
       <c r="E58">
-        <v>452.10169999999999</v>
+        <v>7530.3050000000003</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>7</v>
-      </c>
-      <c r="B59">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B59" s="3">
+        <v>3</v>
       </c>
       <c r="C59" s="1">
-        <v>44761</v>
+        <v>44747</v>
       </c>
       <c r="D59" s="2">
-        <v>0.50069444444444444</v>
+        <v>0.42986111111111108</v>
       </c>
       <c r="E59">
-        <v>491.16950000000003</v>
+        <v>3354.39</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1">
-        <v>44761</v>
+        <v>44750</v>
       </c>
       <c r="D60" s="2">
-        <v>0.5083333333333333</v>
+        <v>0.42638888888888887</v>
       </c>
       <c r="E60">
-        <v>452.18639999999999</v>
+        <v>10517.98</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>8</v>
       </c>
-      <c r="B61" s="3">
-        <v>1</v>
+      <c r="B61">
+        <v>2</v>
       </c>
       <c r="C61" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D61" s="2">
-        <v>0.41111111111111115</v>
+        <v>0.4375</v>
       </c>
       <c r="E61">
-        <v>9397.9320000000007</v>
+        <v>7493.1189999999997</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>8</v>
       </c>
-      <c r="B62" s="3">
-        <v>2</v>
+      <c r="B62">
+        <v>3</v>
       </c>
       <c r="C62" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D62" s="2">
-        <v>0.42222222222222222</v>
+        <v>0.44513888888888892</v>
       </c>
       <c r="E62">
-        <v>7530.3050000000003</v>
+        <v>6369.29</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
-      <c r="B63" s="3">
-        <v>3</v>
+      <c r="B63">
+        <v>1</v>
       </c>
       <c r="C63" s="1">
-        <v>44747</v>
+        <v>44760</v>
       </c>
       <c r="D63" s="2">
-        <v>0.42986111111111108</v>
+        <v>0.42777777777777781</v>
       </c>
       <c r="E63">
-        <v>3354.39</v>
+        <v>5026.1189999999997</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -1509,16 +1517,16 @@
         <v>8</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C64" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D64" s="2">
-        <v>0.42638888888888887</v>
+        <v>0.43541666666666662</v>
       </c>
       <c r="E64">
-        <v>10517.98</v>
+        <v>5242.5590000000002</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -1526,135 +1534,135 @@
         <v>8</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D65" s="2">
-        <v>0.4375</v>
+        <v>0.4458333333333333</v>
       </c>
       <c r="E65">
-        <v>7493.1189999999997</v>
+        <v>4312.1530000000002</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C66" s="1">
+        <v>44747</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.46111111111111108</v>
+      </c>
+      <c r="E66">
+        <v>4119.2879999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3">
+        <v>9</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
+      <c r="C67" s="4">
         <v>44750</v>
       </c>
-      <c r="D66" s="2">
-        <v>0.44513888888888892</v>
-      </c>
-      <c r="E66">
-        <v>6369.29</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>8</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1">
-        <v>44760</v>
-      </c>
-      <c r="D67" s="2">
-        <v>0.42777777777777781</v>
-      </c>
-      <c r="E67">
-        <v>5026.1189999999997</v>
+      <c r="D67" s="5">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="E67" s="3">
+        <v>2890.7629999999999</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>8</v>
-      </c>
-      <c r="B68">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1</v>
       </c>
       <c r="C68" s="1">
         <v>44760</v>
       </c>
       <c r="D68" s="2">
-        <v>0.43541666666666662</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="E68">
-        <v>5242.5590000000002</v>
+        <v>3202.6950000000002</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" s="1">
-        <v>44760</v>
+        <v>44747</v>
       </c>
       <c r="D69" s="2">
-        <v>0.4458333333333333</v>
+        <v>0.48055555555555557</v>
       </c>
       <c r="E69">
-        <v>4312.1530000000002</v>
+        <v>1238.9490000000001</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C70" s="1">
         <v>44747</v>
       </c>
       <c r="D70" s="2">
-        <v>0.46111111111111108</v>
+        <v>0.4916666666666667</v>
       </c>
       <c r="E70">
-        <v>4119.2879999999996</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="3">
-        <v>9</v>
-      </c>
-      <c r="B71" s="3">
-        <v>1</v>
-      </c>
-      <c r="C71" s="4">
-        <v>44750</v>
-      </c>
-      <c r="D71" s="5">
-        <v>0.46736111111111112</v>
-      </c>
-      <c r="E71" s="3">
-        <v>2890.7629999999999</v>
+        <v>1888.932</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1">
+        <v>44747</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E71">
+        <v>2716.78</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>9</v>
-      </c>
-      <c r="B72" s="3">
+        <v>10</v>
+      </c>
+      <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" s="1">
-        <v>44760</v>
+        <v>44750</v>
       </c>
       <c r="D72" s="2">
-        <v>0.41250000000000003</v>
+        <v>0.49236111111111108</v>
       </c>
       <c r="E72">
-        <v>3202.6950000000002</v>
+        <v>1371.4069999999999</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -1662,16 +1670,16 @@
         <v>10</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C73" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D73" s="2">
-        <v>0.48055555555555557</v>
+        <v>0.50069444444444444</v>
       </c>
       <c r="E73">
-        <v>1238.9490000000001</v>
+        <v>2052.39</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -1679,237 +1687,237 @@
         <v>10</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" s="1">
-        <v>44747</v>
+        <v>44750</v>
       </c>
       <c r="D74" s="2">
-        <v>0.4916666666666667</v>
+        <v>0.50624999999999998</v>
       </c>
       <c r="E74">
-        <v>1888.932</v>
+        <v>2159.1689999999999</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>10</v>
       </c>
-      <c r="B75">
-        <v>3</v>
+      <c r="B75" s="3">
+        <v>1</v>
       </c>
       <c r="C75" s="1">
-        <v>44747</v>
+        <v>44760</v>
       </c>
       <c r="D75" s="2">
-        <v>0.5</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="E75">
-        <v>2716.78</v>
+        <v>1568.508</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>10</v>
       </c>
-      <c r="B76">
-        <v>1</v>
+      <c r="B76" s="3">
+        <v>2</v>
       </c>
       <c r="C76" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D76" s="2">
-        <v>0.49236111111111108</v>
+        <v>0.4694444444444445</v>
       </c>
       <c r="E76">
-        <v>1371.4069999999999</v>
+        <v>2633.4749999999999</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
-      <c r="B77">
-        <v>2</v>
+      <c r="B77" s="3">
+        <v>3</v>
       </c>
       <c r="C77" s="1">
-        <v>44750</v>
+        <v>44760</v>
       </c>
       <c r="D77" s="2">
-        <v>0.50069444444444444</v>
+        <v>0.4777777777777778</v>
       </c>
       <c r="E77">
-        <v>2052.39</v>
+        <v>2769.0680000000002</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>10</v>
-      </c>
-      <c r="B78">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1</v>
       </c>
       <c r="C78" s="1">
-        <v>44750</v>
+        <v>44753</v>
       </c>
       <c r="D78" s="2">
-        <v>0.50624999999999998</v>
+        <v>0.47083333333333338</v>
       </c>
       <c r="E78">
-        <v>2159.1689999999999</v>
+        <v>271.01690000000002</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>10</v>
-      </c>
-      <c r="B79" s="3">
+        <v>11</v>
+      </c>
+      <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" s="1">
-        <v>44760</v>
+        <v>44761</v>
       </c>
       <c r="D79" s="2">
-        <v>0.4597222222222222</v>
+        <v>0.50763888888888886</v>
       </c>
       <c r="E79">
-        <v>1568.508</v>
+        <v>453.62709999999998</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>10</v>
-      </c>
-      <c r="B80" s="3">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
       </c>
       <c r="C80" s="1">
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="D80" s="2">
-        <v>0.4694444444444445</v>
+        <v>0.51597222222222217</v>
       </c>
       <c r="E80">
-        <v>2633.4749999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>10</v>
+        <v>456.50850000000003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3">
+        <v>12</v>
       </c>
       <c r="B81" s="3">
-        <v>3</v>
-      </c>
-      <c r="C81" s="1">
-        <v>44760</v>
-      </c>
-      <c r="D81" s="2">
-        <v>0.4777777777777778</v>
-      </c>
-      <c r="E81">
-        <v>2769.0680000000002</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="C81" s="4">
+        <v>44748</v>
+      </c>
+      <c r="D81" s="5">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="E81" s="3">
+        <v>1154.627</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="3">
+        <v>12</v>
       </c>
       <c r="B82" s="3">
-        <v>1</v>
-      </c>
-      <c r="C82" s="1">
-        <v>44753</v>
-      </c>
-      <c r="D82" s="2">
-        <v>0.47083333333333338</v>
-      </c>
-      <c r="E82">
-        <v>271.01690000000002</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>11</v>
-      </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1">
-        <v>44761</v>
-      </c>
-      <c r="D83" s="2">
-        <v>0.50763888888888886</v>
-      </c>
-      <c r="E83">
-        <v>453.62709999999998</v>
+        <v>2</v>
+      </c>
+      <c r="C82" s="4">
+        <v>44748</v>
+      </c>
+      <c r="D82" s="5">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="E82" s="3">
+        <v>1131.7460000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="3">
+        <v>12</v>
+      </c>
+      <c r="B83" s="3">
+        <v>3</v>
+      </c>
+      <c r="C83" s="4">
+        <v>44748</v>
+      </c>
+      <c r="D83" s="5">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="E83" s="3">
+        <v>1113.78</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>11</v>
-      </c>
-      <c r="B84">
+        <v>12</v>
+      </c>
+      <c r="B84" s="3">
         <v>1</v>
       </c>
       <c r="C84" s="1">
         <v>44764</v>
       </c>
       <c r="D84" s="2">
-        <v>0.51597222222222217</v>
+        <v>0.40138888888888885</v>
       </c>
       <c r="E84">
-        <v>456.50850000000003</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="3">
+        <v>834.79629999999997</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85">
         <v>12</v>
       </c>
       <c r="B85" s="3">
-        <v>1</v>
-      </c>
-      <c r="C85" s="4">
-        <v>44748</v>
-      </c>
-      <c r="D85" s="5">
-        <v>0.5180555555555556</v>
-      </c>
-      <c r="E85" s="3">
-        <v>1154.627</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3">
+        <v>2</v>
+      </c>
+      <c r="C85" s="1">
+        <v>44764</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="E85">
+        <v>1625.712</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86">
         <v>12</v>
       </c>
       <c r="B86" s="3">
-        <v>2</v>
-      </c>
-      <c r="C86" s="4">
-        <v>44748</v>
-      </c>
-      <c r="D86" s="5">
-        <v>0.53194444444444444</v>
-      </c>
-      <c r="E86" s="3">
-        <v>1131.7460000000001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="3">
+        <v>3</v>
+      </c>
+      <c r="C86" s="1">
+        <v>44764</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="E86">
+        <v>1475.712</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87">
         <v>12</v>
       </c>
       <c r="B87" s="3">
-        <v>3</v>
-      </c>
-      <c r="C87" s="4">
-        <v>44748</v>
-      </c>
-      <c r="D87" s="5">
-        <v>0.54236111111111118</v>
-      </c>
-      <c r="E87" s="3">
-        <v>1113.78</v>
+        <v>1</v>
+      </c>
+      <c r="C87" s="1">
+        <v>44769</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0.40416666666666662</v>
+      </c>
+      <c r="E87">
+        <v>1459.441</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -1917,16 +1925,16 @@
         <v>12</v>
       </c>
       <c r="B88" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C88" s="1">
-        <v>44764</v>
+        <v>44769</v>
       </c>
       <c r="D88" s="2">
-        <v>0.40138888888888885</v>
+        <v>0.41944444444444445</v>
       </c>
       <c r="E88">
-        <v>834.79629999999997</v>
+        <v>1407.2370000000001</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -1934,94 +1942,26 @@
         <v>12</v>
       </c>
       <c r="B89" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C89" s="1">
-        <v>44764</v>
+        <v>44769</v>
       </c>
       <c r="D89" s="2">
-        <v>0.41250000000000003</v>
+        <v>0.4291666666666667</v>
       </c>
       <c r="E89">
-        <v>1625.712</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>12</v>
-      </c>
-      <c r="B90" s="3">
-        <v>3</v>
-      </c>
-      <c r="C90" s="1">
-        <v>44764</v>
-      </c>
-      <c r="D90" s="2">
-        <v>0.42291666666666666</v>
-      </c>
-      <c r="E90">
-        <v>1475.712</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>12</v>
-      </c>
-      <c r="B91" s="3">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D91" s="2">
-        <v>0.40416666666666662</v>
-      </c>
-      <c r="E91">
-        <v>1459.441</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>12</v>
-      </c>
-      <c r="B92" s="3">
-        <v>2</v>
-      </c>
-      <c r="C92" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D92" s="2">
-        <v>0.41944444444444445</v>
-      </c>
-      <c r="E92">
-        <v>1407.2370000000001</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>12</v>
-      </c>
-      <c r="B93" s="3">
-        <v>3</v>
-      </c>
-      <c r="C93" s="1">
-        <v>44769</v>
-      </c>
-      <c r="D93" s="2">
-        <v>0.4291666666666667</v>
-      </c>
-      <c r="E93">
         <v>1408.0340000000001</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B102" s="3"/>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B98" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wetlands data updated with temperature and water level
</commit_message>
<xml_diff>
--- a/Wetlands/Wetland data.xlsx
+++ b/Wetlands/Wetland data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymad138\Documents\Ecuador2022\Wetlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DC4AEF-C53D-49D5-9023-579BEE55CAA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0F04C-EF65-4ED1-9673-7E04EED2A20A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11020" windowHeight="6280" xr2:uid="{94E7109B-EF61-4772-AC1F-D142A6519923}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>NA</t>
   </si>
   <si>
-    <t xml:space="preserve">Average </t>
+    <t>Standard deviation in ppm per day per wetland</t>
   </si>
   <si>
-    <t>Standard deviation in ppm per day per wetland</t>
+    <t>Average ppm</t>
   </si>
 </sst>
 </file>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF46F0BE-CA28-4568-AEEA-82D636B2E98E}">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,10 +480,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -533,9 +533,13 @@
       <c r="E4" s="3">
         <v>238.81360000000001</v>
       </c>
-      <c r="F4" s="3">
-        <f>_xlfn.VAR.P(E2:E4)</f>
-        <v>0</v>
+      <c r="F4" s="3" t="e">
+        <f>STDEV(E2:E4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="3">
+        <f>AVERAGE(E2:E4)</f>
+        <v>238.81360000000001</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -593,8 +597,8 @@
         <v>24.964284514548631</v>
       </c>
       <c r="G7">
-        <f>VARA(E5:E7)</f>
-        <v>623.21550132333255</v>
+        <f>AVERAGE(E5:E7)</f>
+        <v>349.4539333333334</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -650,8 +654,12 @@
         <v>382.28809999999999</v>
       </c>
       <c r="F10">
-        <f>_xlfn.VAR.P(E8:E10)</f>
-        <v>1423.5797212688901</v>
+        <f>STDEV(E8:E10)</f>
+        <v>46.210059315081331</v>
+      </c>
+      <c r="G10">
+        <f>AVERAGE(E8:E10)</f>
+        <v>408.49153333333334</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -687,6 +695,7 @@
       <c r="E12" s="3">
         <v>224.2373</v>
       </c>
+      <c r="G12"/>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
@@ -702,8 +711,12 @@
         <v>13</v>
       </c>
       <c r="F13" s="3">
-        <f>_xlfn.VAR.P(E11:E12)</f>
-        <v>2.1994373024999749</v>
+        <f>STDEV(E11:E12)</f>
+        <v>2.0973494236774068</v>
+      </c>
+      <c r="G13" s="3">
+        <f>AVERAGE(E11:E12)</f>
+        <v>225.72035</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -757,11 +770,15 @@
         <v>342.01690000000002</v>
       </c>
       <c r="F16">
-        <f>_xlfn.VAR.P(E14:E16)</f>
-        <v>1134.8761138755622</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E14:E16)</f>
+        <v>41.259110155374579</v>
+      </c>
+      <c r="G16">
+        <f>AVERAGE(E14:E16)</f>
+        <v>306.71183333333335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -778,7 +795,7 @@
         <v>290.40679999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -795,7 +812,7 @@
         <v>330.9153</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -812,11 +829,15 @@
         <v>292.18639999999999</v>
       </c>
       <c r="F19">
-        <f>_xlfn.VAR.P(E17:E19)</f>
-        <v>349.33702706888926</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <f>STDEV(E17:E19)</f>
+        <v>22.891167305389516</v>
+      </c>
+      <c r="G19">
+        <f>AVERAGE(E17:E19)</f>
+        <v>304.50283333333329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>3</v>
       </c>
@@ -828,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -842,7 +863,7 @@
         <v>263.22030000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -856,11 +877,15 @@
         <v>275.50850000000003</v>
       </c>
       <c r="F22" s="3">
-        <f>_xlfn.VAR.P(E21:E22)</f>
-        <v>37.749964810000108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E21:E22)</f>
+        <v>8.6890695485765459</v>
+      </c>
+      <c r="G22" s="3">
+        <f>AVERAGE(E21:E22)</f>
+        <v>269.36440000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3</v>
       </c>
@@ -877,7 +902,7 @@
         <v>342.91149999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3</v>
       </c>
@@ -894,7 +919,7 @@
         <v>401.7627</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3</v>
       </c>
@@ -911,11 +936,15 @@
         <v>401.59320000000002</v>
       </c>
       <c r="F25">
-        <f>_xlfn.VAR.P(E23:E25)</f>
-        <v>767.44826517555612</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E23:E25)</f>
+        <v>33.928931574149729</v>
+      </c>
+      <c r="G25">
+        <f>AVERAGE(E23:E25)</f>
+        <v>382.08913333333334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3</v>
       </c>
@@ -932,7 +961,7 @@
         <v>487.61020000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3</v>
       </c>
@@ -949,7 +978,7 @@
         <v>536.33900000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>3</v>
       </c>
@@ -966,11 +995,15 @@
         <v>538.55430000000001</v>
       </c>
       <c r="F28">
-        <f>_xlfn.VAR.P(E26:E28)</f>
-        <v>552.74498092666693</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <f>STDEV(E26:E28)</f>
+        <v>28.794400000520941</v>
+      </c>
+      <c r="G28">
+        <f>AVERAGE(E26:E28)</f>
+        <v>520.83450000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>4</v>
       </c>
@@ -986,12 +1019,16 @@
       <c r="E29" s="3">
         <v>588.96609999999998</v>
       </c>
-      <c r="F29" s="3">
-        <f>_xlfn.VAR.P(E29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="3" t="e">
+        <f>STDEV(E29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="3">
+        <f>AVERAGE(E29)</f>
+        <v>588.96609999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>4</v>
       </c>
@@ -1008,7 +1045,7 @@
         <v>593.62710000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>4</v>
       </c>
@@ -1025,7 +1062,7 @@
         <v>664.72879999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>4</v>
       </c>
@@ -1042,11 +1079,15 @@
         <v>653.79660000000001</v>
       </c>
       <c r="F32" s="3">
-        <f>_xlfn.VAR.P(E30:E32)</f>
-        <v>977.25927444222077</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E30:E32)</f>
+        <v>38.286928731139184</v>
+      </c>
+      <c r="G32" s="3">
+        <f>AVERAGE(E30:E32)</f>
+        <v>637.38416666666672</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1063,7 +1104,7 @@
         <v>395.83049999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1080,7 +1121,7 @@
         <v>492.61020000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1097,11 +1138,15 @@
         <v>492.35590000000002</v>
       </c>
       <c r="F35">
-        <f>_xlfn.VAR.P(E33:E35)</f>
-        <v>2075.9475384155576</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E33:E35)</f>
+        <v>55.802520620697202</v>
+      </c>
+      <c r="G35">
+        <f>AVERAGE(E33:E35)</f>
+        <v>460.26553333333339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1118,7 +1163,7 @@
         <v>756.20699999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1135,7 +1180,7 @@
         <v>681.66629999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1152,11 +1197,15 @@
         <v>669.47460000000001</v>
       </c>
       <c r="F38">
-        <f>_xlfn.VAR.P(E36:E38)</f>
-        <v>1469.7180794599999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E36:E38)</f>
+        <v>46.952924500929647</v>
+      </c>
+      <c r="G38">
+        <f>AVERAGE(E36:E38)</f>
+        <v>702.44929999999988</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
@@ -1172,12 +1221,16 @@
       <c r="E39" s="3">
         <v>459.22030000000001</v>
       </c>
-      <c r="F39">
-        <f>_xlfn.VAR.P(E39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F39" t="e">
+        <f>STDEV(E39)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39">
+        <f>AVERAGE(E39)</f>
+        <v>459.22030000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1194,7 +1247,7 @@
         <v>843.44069999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1211,7 +1264,7 @@
         <v>694.81359999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1228,11 +1281,15 @@
         <v>642.01689999999996</v>
       </c>
       <c r="F42">
-        <f>_xlfn.VAR.P(E40:E42)</f>
-        <v>7272.117065748821</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <f>STDEV(E40:E42)</f>
+        <v>104.44221176623574</v>
+      </c>
+      <c r="G42">
+        <f>AVERAGE(E40:E42)</f>
+        <v>726.75706666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>6</v>
       </c>
@@ -1248,12 +1305,16 @@
       <c r="E43" s="3">
         <v>442.44069999999999</v>
       </c>
-      <c r="F43" s="3">
-        <f>_xlfn.VAR.P(E43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F43" s="3" t="e">
+        <f>STDEV(E43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G43" s="3">
+        <f>AVERAGE(E43)</f>
+        <v>442.44069999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>6</v>
       </c>
@@ -1269,12 +1330,16 @@
       <c r="E44" s="3">
         <v>430.74579999999997</v>
       </c>
-      <c r="F44" s="3">
-        <f>_xlfn.VAR.P(E44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F44" s="3" t="e">
+        <f>STDEV(E44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G44" s="3">
+        <f>AVERAGE(E44)</f>
+        <v>430.74579999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>6</v>
       </c>
@@ -1291,7 +1356,7 @@
         <v>394.05079999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>6</v>
       </c>
@@ -1308,7 +1373,7 @@
         <v>434.89830000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
@@ -1325,11 +1390,15 @@
         <v>393.11860000000001</v>
       </c>
       <c r="F47">
-        <f>_xlfn.VAR.P(E45:E47)</f>
-        <v>379.43673168666675</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <f>STDEV(E45:E47)</f>
+        <v>23.856971675592025</v>
+      </c>
+      <c r="G47">
+        <f>AVERAGE(E45:E47)</f>
+        <v>407.35590000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>7</v>
       </c>
@@ -1346,7 +1415,7 @@
         <v>728.71190000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>7</v>
       </c>
@@ -1363,7 +1432,7 @@
         <v>779.38980000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>7</v>
       </c>
@@ -1380,11 +1449,15 @@
         <v>253.81360000000001</v>
       </c>
       <c r="F50" s="3">
-        <f>_xlfn.VAR.P(E48:E50)</f>
-        <v>56036.331877526623</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <f>STDEV(E48:E50)</f>
+        <v>289.92153734465802</v>
+      </c>
+      <c r="G50" s="3">
+        <f>AVERAGE(E48:E50)</f>
+        <v>587.30510000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7">
         <v>7</v>
       </c>
@@ -1401,7 +1474,7 @@
         <v>268.98309999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7">
         <v>7</v>
       </c>
@@ -1418,7 +1491,7 @@
         <v>225.1695</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="7">
         <v>7</v>
       </c>
@@ -1435,11 +1508,15 @@
         <v>240.8475</v>
       </c>
       <c r="F53" s="7">
-        <f>_xlfn.VAR.P(E51:E53)</f>
-        <v>328.56035736888856</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E51:E53)</f>
+        <v>22.200012073269981</v>
+      </c>
+      <c r="G53" s="7">
+        <f>AVERAGE(E51:E53)</f>
+        <v>245.00003333333333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>7</v>
       </c>
@@ -1456,7 +1533,7 @@
         <v>452.10169999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>7</v>
       </c>
@@ -1473,7 +1550,7 @@
         <v>491.16950000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>7</v>
       </c>
@@ -1490,11 +1567,15 @@
         <v>452.18639999999999</v>
       </c>
       <c r="F56">
-        <f>_xlfn.VAR.P(E54:E56)</f>
-        <v>338.44247294888947</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E54:E56)</f>
+        <v>22.531393863304022</v>
+      </c>
+      <c r="G56">
+        <f>AVERAGE(E54:E56)</f>
+        <v>465.15253333333334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>8</v>
       </c>
@@ -1511,7 +1592,7 @@
         <v>9397.9320000000007</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>8</v>
       </c>
@@ -1528,7 +1609,7 @@
         <v>7530.3050000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1545,11 +1626,15 @@
         <v>3354.39</v>
       </c>
       <c r="F59">
-        <f t="shared" ref="F59:F65" si="0">_xlfn.VAR.P(E57:E59)</f>
-        <v>6383410.7337909006</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E57:E59)</f>
+        <v>3094.368449407139</v>
+      </c>
+      <c r="G59">
+        <f>AVERAGE(E57:E59)</f>
+        <v>6760.8756666666668</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>8</v>
       </c>
@@ -1566,7 +1651,7 @@
         <v>10517.98</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>8</v>
       </c>
@@ -1583,7 +1668,7 @@
         <v>7493.1189999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>8</v>
       </c>
@@ -1603,8 +1688,12 @@
         <f>STDEV(E60:E62)</f>
         <v>2145.7090672107288</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <f>AVERAGE(E60:E62)</f>
+        <v>8126.7963333333328</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -1621,7 +1710,7 @@
         <v>5026.1189999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -1638,7 +1727,7 @@
         <v>5242.5590000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -1655,11 +1744,15 @@
         <v>4312.1530000000002</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
-        <v>158027.67195466658</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E63:E65)</f>
+        <v>486.86908705729087</v>
+      </c>
+      <c r="G65">
+        <f>AVERAGE(E63:E65)</f>
+        <v>4860.277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>9</v>
       </c>
@@ -1675,12 +1768,16 @@
       <c r="E66">
         <v>4119.2879999999996</v>
       </c>
-      <c r="F66">
-        <f>_xlfn.VAR.P(E66)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F66" t="e">
+        <f>STDEV(E66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G66">
+        <f>AVERAGE(E66)</f>
+        <v>4119.2879999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>9</v>
       </c>
@@ -1696,12 +1793,16 @@
       <c r="E67" s="3">
         <v>2890.7629999999999</v>
       </c>
-      <c r="F67">
-        <f>_xlfn.VAR.P(E67)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F67" t="e">
+        <f>STDEV(E67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G68" si="0">AVERAGE(E67)</f>
+        <v>2890.7629999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>9</v>
       </c>
@@ -1717,12 +1818,16 @@
       <c r="E68">
         <v>3202.6950000000002</v>
       </c>
-      <c r="F68">
-        <f>_xlfn.VAR.P(E68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F68" t="e">
+        <f>STDEV(E68)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="0"/>
+        <v>3202.6950000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>10</v>
       </c>
@@ -1739,7 +1844,7 @@
         <v>1238.9490000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>10</v>
       </c>
@@ -1756,7 +1861,7 @@
         <v>1888.932</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>10</v>
       </c>
@@ -1776,8 +1881,12 @@
         <f>STDEV(E69:E71)</f>
         <v>740.6972701396528</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71">
+        <f>AVERAGE(E69:E71)</f>
+        <v>1948.2203333333334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>10</v>
       </c>
@@ -1794,7 +1903,7 @@
         <v>1371.4069999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>10</v>
       </c>
@@ -1811,7 +1920,7 @@
         <v>2052.39</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>10</v>
       </c>
@@ -1828,11 +1937,15 @@
         <v>2159.1689999999999</v>
       </c>
       <c r="F74">
-        <f t="shared" ref="F74:F77" si="1">_xlfn.VAR.P(E72:E74)</f>
-        <v>121745.39664155534</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E72:E74)</f>
+        <v>427.33838461146144</v>
+      </c>
+      <c r="G74">
+        <f>AVERAGE(E72:E74)</f>
+        <v>1860.9886666666664</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>10</v>
       </c>
@@ -1849,7 +1962,7 @@
         <v>1568.508</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>10</v>
       </c>
@@ -1866,7 +1979,7 @@
         <v>2633.4749999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>10</v>
       </c>
@@ -1883,11 +1996,15 @@
         <v>2769.0680000000002</v>
       </c>
       <c r="F77">
-        <f t="shared" si="1"/>
-        <v>288209.38737088774</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E75:E77)</f>
+        <v>657.5059551489494</v>
+      </c>
+      <c r="G77">
+        <f>AVERAGE(E75:E77)</f>
+        <v>2323.6836666666668</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>11</v>
       </c>
@@ -1903,12 +2020,16 @@
       <c r="E78">
         <v>271.01690000000002</v>
       </c>
-      <c r="F78">
-        <f>_xlfn.VAR.P(E78)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F78" t="e">
+        <f>STDEV(E78)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G78">
+        <f>AVERAGE(E78)</f>
+        <v>271.01690000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>11</v>
       </c>
@@ -1924,12 +2045,16 @@
       <c r="E79">
         <v>453.62709999999998</v>
       </c>
-      <c r="F79">
-        <f t="shared" ref="F79:F80" si="2">_xlfn.VAR.P(E79)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F79" t="e">
+        <f t="shared" ref="F79:G80" si="1">STDEV(E79)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G79">
+        <f t="shared" ref="G79:G80" si="2">AVERAGE(E79)</f>
+        <v>453.62709999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>11</v>
       </c>
@@ -1945,12 +2070,16 @@
       <c r="E80">
         <v>456.50850000000003</v>
       </c>
-      <c r="F80">
+      <c r="F80" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G80">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>456.50850000000003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>12</v>
       </c>
@@ -1967,7 +2096,7 @@
         <v>1154.627</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>12</v>
       </c>
@@ -1984,7 +2113,7 @@
         <v>1131.7460000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>12</v>
       </c>
@@ -2001,11 +2130,15 @@
         <v>1113.78</v>
       </c>
       <c r="F83" s="3">
-        <f>_xlfn.VAR.P(E81:E83)</f>
-        <v>279.42163622222182</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E81:E83)</f>
+        <v>20.472724643616264</v>
+      </c>
+      <c r="G83" s="3">
+        <f>AVERAGE(E81:E83)</f>
+        <v>1133.3843333333334</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>12</v>
       </c>
@@ -2022,8 +2155,9 @@
         <v>834.79629999999997</v>
       </c>
       <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>12</v>
       </c>
@@ -2040,8 +2174,9 @@
         <v>1625.712</v>
       </c>
       <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>12</v>
       </c>
@@ -2058,11 +2193,15 @@
         <v>1475.712</v>
       </c>
       <c r="F86" s="3">
-        <f t="shared" ref="F86:F89" si="3">_xlfn.VAR.P(E84:E86)</f>
-        <v>117646.7310014423</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E84:E86)</f>
+        <v>420.08343992850212</v>
+      </c>
+      <c r="G86" s="3">
+        <f>AVERAGE(E84:E86)</f>
+        <v>1312.0734333333332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>12</v>
       </c>
@@ -2079,8 +2218,9 @@
         <v>1459.441</v>
       </c>
       <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>12</v>
       </c>
@@ -2097,8 +2237,9 @@
         <v>1407.2370000000001</v>
       </c>
       <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>12</v>
       </c>
@@ -2115,11 +2256,15 @@
         <v>1408.0340000000001</v>
       </c>
       <c r="F89" s="3">
-        <f t="shared" si="3"/>
-        <v>596.50805266666532</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+        <f>STDEV(E87:E89)</f>
+        <v>29.912573928032305</v>
+      </c>
+      <c r="G89" s="3">
+        <f>AVERAGE(E7:E89)</f>
+        <v>1510.4936234567901</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B96" s="3"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>